<commit_message>
added info in systemicWrongButtons
</commit_message>
<xml_diff>
--- a/behavioral/REV_SST/info/systematicWrongButtons.xlsx
+++ b/behavioral/REV_SST/info/systematicWrongButtons.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV/REV_SST/info/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>NaN</t>
   </si>
@@ -58,15 +53,37 @@
   <si>
     <t>82</t>
   </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,8 +106,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -100,7 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -156,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -191,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -368,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,18 +405,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="3">
         <v>6</v>
       </c>
@@ -401,7 +430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="3">
         <v>6</v>
       </c>
@@ -415,7 +444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -429,7 +458,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>7</v>
       </c>
@@ -443,7 +472,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>8</v>
       </c>
@@ -457,7 +486,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>9</v>
       </c>
@@ -471,7 +500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>9</v>
       </c>
@@ -485,7 +514,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>12</v>
       </c>
@@ -499,7 +528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -513,7 +542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>15</v>
       </c>
@@ -527,7 +556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
         <v>25</v>
       </c>
@@ -541,7 +570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,7 +584,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
         <v>28</v>
       </c>
@@ -569,7 +598,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -583,7 +612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
         <v>33</v>
       </c>
@@ -597,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>36</v>
       </c>
@@ -611,7 +640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="4">
         <v>40</v>
       </c>
@@ -625,7 +654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="2" customFormat="1">
       <c r="A18" s="4">
         <v>41</v>
       </c>
@@ -639,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" s="2" customFormat="1">
       <c r="A19" s="4">
         <v>42</v>
       </c>
@@ -653,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="2" customFormat="1">
       <c r="A20" s="5">
         <v>100</v>
       </c>
@@ -667,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="4">
         <v>116</v>
       </c>
@@ -681,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="4">
         <v>116</v>
       </c>
@@ -695,7 +724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="4">
         <v>116</v>
       </c>
@@ -709,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="4">
         <v>116</v>
       </c>
@@ -723,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="4">
         <v>116</v>
       </c>
@@ -737,7 +766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="4">
         <v>116</v>
       </c>
@@ -751,7 +780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="4">
         <v>116</v>
       </c>
@@ -765,7 +794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="4">
         <v>138</v>
       </c>
@@ -779,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="4">
         <v>142</v>
       </c>
@@ -793,7 +822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="4">
         <v>118</v>
       </c>
@@ -807,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -821,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -835,7 +864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -849,7 +878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -863,7 +892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -877,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -891,7 +920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
@@ -905,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -919,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -933,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -947,7 +976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -961,7 +990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -975,7 +1004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -989,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
@@ -1031,7 +1060,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="4">
         <v>36</v>
       </c>
@@ -1045,7 +1074,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="4">
         <v>36</v>
       </c>
@@ -1059,7 +1088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="4">
         <v>36</v>
       </c>
@@ -1073,7 +1102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4">
         <v>36</v>
       </c>
@@ -1087,7 +1116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4">
         <v>36</v>
       </c>
@@ -1101,7 +1130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="4">
         <v>36</v>
       </c>
@@ -1115,7 +1144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4">
         <v>36</v>
       </c>
@@ -1129,7 +1158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4">
         <v>36</v>
       </c>
@@ -1143,7 +1172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1157,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>9</v>
       </c>
@@ -1213,7 +1242,153 @@
         <v>21</v>
       </c>
     </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>197</v>
+      </c>
+      <c r="D60">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>15</v>
+      </c>
+      <c r="D63">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <v>15</v>
+      </c>
+      <c r="D66">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added txt files with path names to be used for file size correction
</commit_message>
<xml_diff>
--- a/behavioral/REV_SST/info/systematicWrongButtons.xlsx
+++ b/behavioral/REV_SST/info/systematicWrongButtons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -640,26 +640,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" s="2" customFormat="1">
       <c r="A17" s="4">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1">
       <c r="A18" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
@@ -669,11 +669,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1">
-      <c r="A19" s="4">
-        <v>42</v>
+      <c r="A19" s="5">
+        <v>100</v>
       </c>
       <c r="B19" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
@@ -682,18 +682,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1">
-      <c r="A20" s="5">
-        <v>100</v>
-      </c>
-      <c r="B20" s="2">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>0</v>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4">
+        <v>116</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -701,7 +701,7 @@
         <v>116</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -715,7 +715,7 @@
         <v>116</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -729,7 +729,7 @@
         <v>116</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -743,7 +743,7 @@
         <v>116</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -757,7 +757,7 @@
         <v>116</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -771,7 +771,7 @@
         <v>116</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>15</v>
@@ -782,10 +782,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -796,10 +796,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -810,30 +810,30 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4">
-        <v>118</v>
+      <c r="A30" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>0</v>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31">
         <v>15</v>
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <v>15</v>
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33">
         <v>15</v>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>15</v>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <v>15</v>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36">
         <v>15</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>15</v>
@@ -939,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>15</v>
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C39">
         <v>15</v>
@@ -967,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C40">
         <v>15</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>15</v>
@@ -995,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C42">
         <v>15</v>
@@ -1009,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C43">
         <v>15</v>
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>15</v>
@@ -1034,30 +1034,30 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>91</v>
+      </c>
+      <c r="D45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4">
+        <v>36</v>
+      </c>
+      <c r="B46">
         <v>4</v>
       </c>
-      <c r="B45">
-        <v>12</v>
-      </c>
-      <c r="C45">
-        <v>15</v>
-      </c>
-      <c r="D45">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46">
-        <v>14</v>
-      </c>
       <c r="C46">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D46">
-        <v>95</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1065,7 +1065,7 @@
         <v>36</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -1079,7 +1079,7 @@
         <v>36</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48">
         <v>15</v>
@@ -1093,7 +1093,7 @@
         <v>36</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -1107,7 +1107,7 @@
         <v>36</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C50">
         <v>15</v>
@@ -1121,7 +1121,7 @@
         <v>36</v>
       </c>
       <c r="B51">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C51">
         <v>15</v>
@@ -1135,7 +1135,7 @@
         <v>36</v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52">
         <v>15</v>
@@ -1149,7 +1149,7 @@
         <v>36</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C53">
         <v>15</v>
@@ -1159,11 +1159,11 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="4">
-        <v>36</v>
+      <c r="A54" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>15</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C58">
         <v>15</v>
@@ -1230,30 +1230,30 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="D59">
-        <v>21</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C60">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="D60">
-        <v>198</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1261,7 +1261,7 @@
         <v>11</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61">
         <v>15</v>
@@ -1275,7 +1275,7 @@
         <v>11</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>15</v>
@@ -1289,7 +1289,7 @@
         <v>11</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C63">
         <v>15</v>
@@ -1303,7 +1303,7 @@
         <v>11</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64">
         <v>15</v>
@@ -1317,7 +1317,7 @@
         <v>11</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C65">
         <v>15</v>
@@ -1331,7 +1331,7 @@
         <v>11</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C66">
         <v>15</v>
@@ -1345,7 +1345,7 @@
         <v>11</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C67">
         <v>15</v>
@@ -1359,26 +1359,12 @@
         <v>11</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C68">
         <v>15</v>
       </c>
       <c r="D68">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69">
-        <v>12</v>
-      </c>
-      <c r="C69">
-        <v>15</v>
-      </c>
-      <c r="D69">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add info for REV051 and REV138 to systematicWrongButtons.txt. These participants were using 91 for right and 94 for left and so had accumulated a lot of Failed Gos
</commit_message>
<xml_diff>
--- a/behavioral/REV_SST/info/systematicWrongButtons.xlsx
+++ b/behavioral/REV_SST/info/systematicWrongButtons.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendancullen/Library/Containers/com.microsoft.Excel/Data/Desktop/REV_scripts/behavioral/REV_SST/info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09845DB1-32E5-1844-99DA-8D206ED4FF77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19580" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
   <si>
     <t>NaN</t>
   </si>
@@ -59,11 +65,14 @@
   <si>
     <t>112</t>
   </si>
+  <si>
+    <t>138</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -137,6 +146,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -397,26 +409,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
         <v>6</v>
       </c>
@@ -430,7 +442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>6</v>
       </c>
@@ -444,7 +456,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -458,7 +470,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>7</v>
       </c>
@@ -472,7 +484,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>8</v>
       </c>
@@ -486,7 +498,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>9</v>
       </c>
@@ -500,7 +512,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>9</v>
       </c>
@@ -514,7 +526,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>12</v>
       </c>
@@ -528,7 +540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -542,7 +554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>15</v>
       </c>
@@ -556,7 +568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>25</v>
       </c>
@@ -570,7 +582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -584,7 +596,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>28</v>
       </c>
@@ -598,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -612,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>33</v>
       </c>
@@ -626,7 +638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>36</v>
       </c>
@@ -640,7 +652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1">
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>41</v>
       </c>
@@ -654,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1">
+    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>42</v>
       </c>
@@ -668,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="2" customFormat="1">
+    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>100</v>
       </c>
@@ -682,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>116</v>
       </c>
@@ -696,7 +708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>116</v>
       </c>
@@ -710,7 +722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>116</v>
       </c>
@@ -724,7 +736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>116</v>
       </c>
@@ -738,7 +750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>116</v>
       </c>
@@ -752,7 +764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>116</v>
       </c>
@@ -766,7 +778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>116</v>
       </c>
@@ -780,7 +792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>138</v>
       </c>
@@ -794,7 +806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>142</v>
       </c>
@@ -808,7 +820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>118</v>
       </c>
@@ -822,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -836,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -850,7 +862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -864,7 +876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -878,7 +890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -892,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -906,7 +918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -920,7 +932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -934,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -948,7 +960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -962,7 +974,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -976,40 +988,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="D41">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="D42">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C43">
         <v>15</v>
@@ -1018,68 +1030,68 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
         <v>12</v>
       </c>
-      <c r="C44">
-        <v>15</v>
-      </c>
-      <c r="D44">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
+      <c r="C46">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>14</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>91</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4">
-        <v>36</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>15</v>
-      </c>
-      <c r="D46">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="4">
-        <v>36</v>
-      </c>
-      <c r="B47">
-        <v>5</v>
-      </c>
-      <c r="C47">
-        <v>15</v>
-      </c>
-      <c r="D47">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>36</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>15</v>
@@ -1088,12 +1100,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>36</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -1102,12 +1114,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>36</v>
       </c>
       <c r="B50">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>15</v>
@@ -1116,12 +1128,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>36</v>
       </c>
       <c r="B51">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>15</v>
@@ -1130,12 +1142,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>36</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C52">
         <v>15</v>
@@ -1144,51 +1156,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>36</v>
       </c>
       <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>36</v>
+      </c>
+      <c r="B54">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>36</v>
+      </c>
+      <c r="B55">
         <v>12</v>
       </c>
-      <c r="C53">
-        <v>15</v>
-      </c>
-      <c r="D53">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
+      <c r="C55">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54">
-        <v>15</v>
-      </c>
-      <c r="D54">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
-      </c>
-      <c r="C55">
-        <v>15</v>
-      </c>
-      <c r="D55">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -1200,9 +1212,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -1214,12 +1226,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>15</v>
@@ -1228,54 +1240,54 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
         <v>197</v>
       </c>
-      <c r="D59">
+      <c r="D61">
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61">
-        <v>5</v>
-      </c>
-      <c r="C61">
-        <v>15</v>
-      </c>
-      <c r="D61">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>15</v>
@@ -1284,12 +1296,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C63">
         <v>15</v>
@@ -1298,12 +1310,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B64">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>15</v>
@@ -1312,12 +1324,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C65">
         <v>15</v>
@@ -1326,12 +1338,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B66">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C66">
         <v>15</v>
@@ -1340,12 +1352,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67">
         <v>15</v>
@@ -1354,18 +1366,74 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B68">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70">
         <v>12</v>
       </c>
-      <c r="C68">
-        <v>15</v>
-      </c>
-      <c r="D68">
-        <v>21</v>
+      <c r="C70">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>94</v>
+      </c>
+      <c r="D71">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>94</v>
+      </c>
+      <c r="D72">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>